<commit_message>
Updated graphs with new serie TotalAmount
</commit_message>
<xml_diff>
--- a/src/data/kpis.xlsx
+++ b/src/data/kpis.xlsx
@@ -1886,7 +1886,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart173.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart216.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2161,11 +2161,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="84174642"/>
-        <c:axId val="76477354"/>
+        <c:axId val="32569599"/>
+        <c:axId val="39187634"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84174642"/>
+        <c:axId val="32569599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,7 +2197,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76477354"/>
+        <c:crossAx val="39187634"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2205,7 +2205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76477354"/>
+        <c:axId val="39187634"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -2246,7 +2246,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84174642"/>
+        <c:crossAx val="32569599"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2298,7 +2298,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart174.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart217.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2573,11 +2573,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="92093495"/>
-        <c:axId val="60909077"/>
+        <c:axId val="83873322"/>
+        <c:axId val="63884399"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92093495"/>
+        <c:axId val="83873322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,7 +2609,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60909077"/>
+        <c:crossAx val="63884399"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2617,7 +2617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60909077"/>
+        <c:axId val="63884399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="700"/>
@@ -2658,7 +2658,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92093495"/>
+        <c:crossAx val="83873322"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2710,7 +2710,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart175.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart218.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2993,11 +2993,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="916649"/>
-        <c:axId val="20410880"/>
+        <c:axId val="97414840"/>
+        <c:axId val="29768414"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="916649"/>
+        <c:axId val="97414840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3029,7 +3029,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20410880"/>
+        <c:crossAx val="29768414"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3037,7 +3037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20410880"/>
+        <c:axId val="29768414"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3076,7 +3076,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="916649"/>
+        <c:crossAx val="97414840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3128,7 +3128,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart176.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart219.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3403,11 +3403,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="39801258"/>
-        <c:axId val="12914083"/>
+        <c:axId val="8028855"/>
+        <c:axId val="12510566"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39801258"/>
+        <c:axId val="8028855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3439,7 +3439,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12914083"/>
+        <c:crossAx val="12510566"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3447,7 +3447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12914083"/>
+        <c:axId val="12510566"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3487,7 +3487,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39801258"/>
+        <c:crossAx val="8028855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3539,7 +3539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart177.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart220.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4015,11 +4015,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="21532548"/>
-        <c:axId val="12850724"/>
+        <c:axId val="27664461"/>
+        <c:axId val="60875798"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="21532548"/>
+        <c:axId val="27664461"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4051,7 +4051,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12850724"/>
+        <c:crossAx val="60875798"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4059,7 +4059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12850724"/>
+        <c:axId val="60875798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -4099,7 +4099,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21532548"/>
+        <c:crossAx val="27664461"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4152,7 +4152,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart178.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart221.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4628,11 +4628,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="64471947"/>
-        <c:axId val="10756960"/>
+        <c:axId val="45567183"/>
+        <c:axId val="71621298"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64471947"/>
+        <c:axId val="45567183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4664,7 +4664,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10756960"/>
+        <c:crossAx val="71621298"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4672,7 +4672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10756960"/>
+        <c:axId val="71621298"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -4713,7 +4713,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64471947"/>
+        <c:crossAx val="45567183"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4765,7 +4765,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart179.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart222.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5241,11 +5241,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="55448946"/>
-        <c:axId val="77747833"/>
+        <c:axId val="9334544"/>
+        <c:axId val="45252486"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55448946"/>
+        <c:axId val="9334544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5277,7 +5277,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77747833"/>
+        <c:crossAx val="45252486"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5285,7 +5285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77747833"/>
+        <c:axId val="45252486"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5324,7 +5324,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55448946"/>
+        <c:crossAx val="9334544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5376,7 +5376,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart180.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart223.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5852,11 +5852,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="99054807"/>
-        <c:axId val="31098715"/>
+        <c:axId val="29170319"/>
+        <c:axId val="88915788"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99054807"/>
+        <c:axId val="29170319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5888,7 +5888,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31098715"/>
+        <c:crossAx val="88915788"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5896,7 +5896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31098715"/>
+        <c:axId val="88915788"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5936,7 +5936,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99054807"/>
+        <c:crossAx val="29170319"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5988,7 +5988,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart181.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart224.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6464,11 +6464,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="47569660"/>
-        <c:axId val="75438766"/>
+        <c:axId val="92361933"/>
+        <c:axId val="36145061"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47569660"/>
+        <c:axId val="92361933"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6500,7 +6500,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75438766"/>
+        <c:crossAx val="36145061"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6508,7 +6508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75438766"/>
+        <c:axId val="36145061"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -6548,7 +6548,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47569660"/>
+        <c:crossAx val="92361933"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6600,7 +6600,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart182.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart225.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7076,11 +7076,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="51830499"/>
-        <c:axId val="9000682"/>
+        <c:axId val="90286094"/>
+        <c:axId val="74342720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51830499"/>
+        <c:axId val="90286094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7112,7 +7112,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9000682"/>
+        <c:crossAx val="74342720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7120,7 +7120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9000682"/>
+        <c:axId val="74342720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -7160,7 +7160,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51830499"/>
+        <c:crossAx val="90286094"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7212,7 +7212,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart183.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart226.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7688,11 +7688,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="3573401"/>
-        <c:axId val="65316081"/>
+        <c:axId val="80210936"/>
+        <c:axId val="7805634"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3573401"/>
+        <c:axId val="80210936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7724,7 +7724,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65316081"/>
+        <c:crossAx val="7805634"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7732,7 +7732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65316081"/>
+        <c:axId val="7805634"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -7772,7 +7772,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3573401"/>
+        <c:crossAx val="80210936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7825,7 +7825,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart184.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart227.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8301,11 +8301,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="46545188"/>
-        <c:axId val="82355892"/>
+        <c:axId val="66238845"/>
+        <c:axId val="9018891"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46545188"/>
+        <c:axId val="66238845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8337,7 +8337,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82355892"/>
+        <c:crossAx val="9018891"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8345,7 +8345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82355892"/>
+        <c:axId val="9018891"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8384,7 +8384,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46545188"/>
+        <c:crossAx val="66238845"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8437,7 +8437,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart185.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart228.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8913,11 +8913,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="27469696"/>
-        <c:axId val="40808841"/>
+        <c:axId val="36848202"/>
+        <c:axId val="69820115"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="27469696"/>
+        <c:axId val="36848202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8949,7 +8949,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40808841"/>
+        <c:crossAx val="69820115"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8957,7 +8957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40808841"/>
+        <c:axId val="69820115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -8997,7 +8997,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27469696"/>
+        <c:crossAx val="36848202"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9049,7 +9049,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart186.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart229.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9525,11 +9525,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="57839120"/>
-        <c:axId val="28110835"/>
+        <c:axId val="72481466"/>
+        <c:axId val="14285423"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57839120"/>
+        <c:axId val="72481466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9561,7 +9561,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28110835"/>
+        <c:crossAx val="14285423"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9569,7 +9569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28110835"/>
+        <c:axId val="14285423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -9610,7 +9610,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57839120"/>
+        <c:crossAx val="72481466"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9662,7 +9662,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart187.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart230.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -10138,11 +10138,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2292631"/>
-        <c:axId val="51607255"/>
+        <c:axId val="78760947"/>
+        <c:axId val="51562857"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2292631"/>
+        <c:axId val="78760947"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10174,7 +10174,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51607255"/>
+        <c:crossAx val="51562857"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10182,7 +10182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51607255"/>
+        <c:axId val="51562857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -10222,7 +10222,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2292631"/>
+        <c:crossAx val="78760947"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -10276,7 +10276,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart188.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart231.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -10752,11 +10752,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="23548217"/>
-        <c:axId val="59427606"/>
+        <c:axId val="88549874"/>
+        <c:axId val="78471435"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23548217"/>
+        <c:axId val="88549874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10788,7 +10788,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59427606"/>
+        <c:crossAx val="78471435"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10796,7 +10796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59427606"/>
+        <c:axId val="78471435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -10837,7 +10837,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23548217"/>
+        <c:crossAx val="88549874"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10890,7 +10890,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart189.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart232.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11183,11 +11183,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="60758468"/>
-        <c:axId val="19570055"/>
+        <c:axId val="67663709"/>
+        <c:axId val="43244400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60758468"/>
+        <c:axId val="67663709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11219,7 +11219,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19570055"/>
+        <c:crossAx val="43244400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11227,7 +11227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19570055"/>
+        <c:axId val="43244400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -11267,7 +11267,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60758468"/>
+        <c:crossAx val="67663709"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11319,7 +11319,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart190.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart233.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11612,11 +11612,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="30313873"/>
-        <c:axId val="80077433"/>
+        <c:axId val="91415778"/>
+        <c:axId val="49402250"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="30313873"/>
+        <c:axId val="91415778"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11648,7 +11648,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80077433"/>
+        <c:crossAx val="49402250"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11656,7 +11656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80077433"/>
+        <c:axId val="49402250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11695,7 +11695,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30313873"/>
+        <c:crossAx val="91415778"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11747,7 +11747,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart191.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart234.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12184,11 +12184,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="16846990"/>
-        <c:axId val="54621518"/>
+        <c:axId val="2149873"/>
+        <c:axId val="73250283"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="16846990"/>
+        <c:axId val="2149873"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12220,7 +12220,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54621518"/>
+        <c:crossAx val="73250283"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12228,7 +12228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54621518"/>
+        <c:axId val="73250283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12267,7 +12267,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16846990"/>
+        <c:crossAx val="2149873"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12319,7 +12319,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart192.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart235.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12756,11 +12756,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="64167306"/>
-        <c:axId val="27643985"/>
+        <c:axId val="47957986"/>
+        <c:axId val="55305897"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64167306"/>
+        <c:axId val="47957986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12792,7 +12792,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27643985"/>
+        <c:crossAx val="55305897"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12800,7 +12800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27643985"/>
+        <c:axId val="55305897"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12839,7 +12839,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64167306"/>
+        <c:crossAx val="47957986"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12891,7 +12891,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart193.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart236.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13328,11 +13328,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="65327760"/>
-        <c:axId val="78277312"/>
+        <c:axId val="54290325"/>
+        <c:axId val="82886856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65327760"/>
+        <c:axId val="54290325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13364,7 +13364,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78277312"/>
+        <c:crossAx val="82886856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13372,7 +13372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78277312"/>
+        <c:axId val="82886856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13411,7 +13411,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65327760"/>
+        <c:crossAx val="54290325"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13463,7 +13463,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart194.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart237.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13900,11 +13900,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="87356895"/>
-        <c:axId val="75158422"/>
+        <c:axId val="66088190"/>
+        <c:axId val="96209706"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87356895"/>
+        <c:axId val="66088190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13936,7 +13936,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75158422"/>
+        <c:crossAx val="96209706"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13944,7 +13944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75158422"/>
+        <c:axId val="96209706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13983,7 +13983,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87356895"/>
+        <c:crossAx val="66088190"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14035,7 +14035,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart195.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart238.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -14472,11 +14472,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="68850307"/>
-        <c:axId val="20636751"/>
+        <c:axId val="71682503"/>
+        <c:axId val="17598986"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68850307"/>
+        <c:axId val="71682503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14508,7 +14508,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20636751"/>
+        <c:crossAx val="17598986"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14516,7 +14516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20636751"/>
+        <c:axId val="17598986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14555,7 +14555,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68850307"/>
+        <c:crossAx val="71682503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14607,7 +14607,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart196.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart239.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15044,11 +15044,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="20528865"/>
-        <c:axId val="35926000"/>
+        <c:axId val="80404680"/>
+        <c:axId val="60895655"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="20528865"/>
+        <c:axId val="80404680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15080,7 +15080,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35926000"/>
+        <c:crossAx val="60895655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15088,7 +15088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35926000"/>
+        <c:axId val="60895655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -15128,7 +15128,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20528865"/>
+        <c:crossAx val="80404680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15180,7 +15180,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart197.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart240.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15617,11 +15617,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="53134229"/>
-        <c:axId val="1470857"/>
+        <c:axId val="94725016"/>
+        <c:axId val="66218345"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53134229"/>
+        <c:axId val="94725016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15653,7 +15653,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1470857"/>
+        <c:crossAx val="66218345"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15661,7 +15661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1470857"/>
+        <c:axId val="66218345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15700,7 +15700,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53134229"/>
+        <c:crossAx val="94725016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15752,7 +15752,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart198.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart241.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -16189,11 +16189,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="16723232"/>
-        <c:axId val="12579805"/>
+        <c:axId val="90922522"/>
+        <c:axId val="23604019"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="16723232"/>
+        <c:axId val="90922522"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16225,7 +16225,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12579805"/>
+        <c:crossAx val="23604019"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16233,7 +16233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12579805"/>
+        <c:axId val="23604019"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -16273,7 +16273,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16723232"/>
+        <c:crossAx val="90922522"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16325,7 +16325,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart199.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart242.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -16698,11 +16698,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="85543560"/>
-        <c:axId val="66942052"/>
+        <c:axId val="37707798"/>
+        <c:axId val="74521847"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85543560"/>
+        <c:axId val="37707798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16734,7 +16734,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66942052"/>
+        <c:crossAx val="74521847"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16742,7 +16742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66942052"/>
+        <c:axId val="74521847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -16782,7 +16782,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85543560"/>
+        <c:crossAx val="37707798"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16834,7 +16834,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart200.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart243.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -17207,11 +17207,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="82360614"/>
-        <c:axId val="65567641"/>
+        <c:axId val="50497564"/>
+        <c:axId val="44377059"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82360614"/>
+        <c:axId val="50497564"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17243,7 +17243,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65567641"/>
+        <c:crossAx val="44377059"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17251,7 +17251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65567641"/>
+        <c:axId val="44377059"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -17291,7 +17291,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82360614"/>
+        <c:crossAx val="50497564"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17343,7 +17343,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart201.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart244.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -17716,11 +17716,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="47795920"/>
-        <c:axId val="426133"/>
+        <c:axId val="44995518"/>
+        <c:axId val="10893271"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47795920"/>
+        <c:axId val="44995518"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17752,7 +17752,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="426133"/>
+        <c:crossAx val="10893271"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17760,7 +17760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426133"/>
+        <c:axId val="10893271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -17800,7 +17800,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47795920"/>
+        <c:crossAx val="44995518"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17852,7 +17852,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart202.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart245.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -18225,11 +18225,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="77795711"/>
-        <c:axId val="71393430"/>
+        <c:axId val="33550171"/>
+        <c:axId val="28384355"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77795711"/>
+        <c:axId val="33550171"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18261,7 +18261,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71393430"/>
+        <c:crossAx val="28384355"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18269,7 +18269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71393430"/>
+        <c:axId val="28384355"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18308,7 +18308,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77795711"/>
+        <c:crossAx val="33550171"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18360,7 +18360,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart203.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart246.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -18733,11 +18733,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="46916532"/>
-        <c:axId val="92530483"/>
+        <c:axId val="9132523"/>
+        <c:axId val="7813793"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46916532"/>
+        <c:axId val="9132523"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18769,7 +18769,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92530483"/>
+        <c:crossAx val="7813793"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18777,7 +18777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92530483"/>
+        <c:axId val="7813793"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18816,7 +18816,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46916532"/>
+        <c:crossAx val="9132523"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18868,7 +18868,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart204.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart247.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -19241,11 +19241,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="99466939"/>
-        <c:axId val="57828994"/>
+        <c:axId val="4913168"/>
+        <c:axId val="66857414"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99466939"/>
+        <c:axId val="4913168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19277,7 +19277,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57828994"/>
+        <c:crossAx val="66857414"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19285,7 +19285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57828994"/>
+        <c:axId val="66857414"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19324,7 +19324,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99466939"/>
+        <c:crossAx val="4913168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19376,7 +19376,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart205.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart248.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -19651,11 +19651,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="2803033"/>
-        <c:axId val="70557618"/>
+        <c:axId val="4448028"/>
+        <c:axId val="74863438"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2803033"/>
+        <c:axId val="4448028"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19687,7 +19687,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70557618"/>
+        <c:crossAx val="74863438"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19695,7 +19695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70557618"/>
+        <c:axId val="74863438"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -19736,7 +19736,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2803033"/>
+        <c:crossAx val="4448028"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19789,7 +19789,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart206.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart249.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -20064,11 +20064,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="65718943"/>
-        <c:axId val="64249668"/>
+        <c:axId val="15288458"/>
+        <c:axId val="33814243"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65718943"/>
+        <c:axId val="15288458"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20100,7 +20100,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64249668"/>
+        <c:crossAx val="33814243"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20108,7 +20108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64249668"/>
+        <c:axId val="33814243"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -20148,7 +20148,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65718943"/>
+        <c:crossAx val="15288458"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20201,7 +20201,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart207.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart250.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -20476,11 +20476,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="14433531"/>
-        <c:axId val="12264845"/>
+        <c:axId val="18771910"/>
+        <c:axId val="65108747"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14433531"/>
+        <c:axId val="18771910"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20512,7 +20512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12264845"/>
+        <c:crossAx val="65108747"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20520,7 +20520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12264845"/>
+        <c:axId val="65108747"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -20561,7 +20561,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14433531"/>
+        <c:crossAx val="18771910"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20614,7 +20614,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart208.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart251.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -20889,11 +20889,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="66010309"/>
-        <c:axId val="10684752"/>
+        <c:axId val="7987983"/>
+        <c:axId val="44443372"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66010309"/>
+        <c:axId val="7987983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20925,7 +20925,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10684752"/>
+        <c:crossAx val="44443372"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20933,7 +20933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10684752"/>
+        <c:axId val="44443372"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -20973,7 +20973,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66010309"/>
+        <c:crossAx val="7987983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21025,7 +21025,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart209.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart252.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21300,11 +21300,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="26905506"/>
-        <c:axId val="41135191"/>
+        <c:axId val="62146196"/>
+        <c:axId val="86164803"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="26905506"/>
+        <c:axId val="62146196"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21336,7 +21336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41135191"/>
+        <c:crossAx val="86164803"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21344,7 +21344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41135191"/>
+        <c:axId val="86164803"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -21385,7 +21385,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26905506"/>
+        <c:crossAx val="62146196"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21437,7 +21437,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart210.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart253.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21712,11 +21712,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="39246878"/>
-        <c:axId val="68856686"/>
+        <c:axId val="61582262"/>
+        <c:axId val="57368704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39246878"/>
+        <c:axId val="61582262"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21748,7 +21748,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68856686"/>
+        <c:crossAx val="57368704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21756,7 +21756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68856686"/>
+        <c:axId val="57368704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -21796,7 +21796,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39246878"/>
+        <c:crossAx val="61582262"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21848,7 +21848,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart211.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart254.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -22123,11 +22123,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="23476956"/>
-        <c:axId val="68942606"/>
+        <c:axId val="18001325"/>
+        <c:axId val="8636981"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23476956"/>
+        <c:axId val="18001325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22159,7 +22159,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68942606"/>
+        <c:crossAx val="8636981"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22167,7 +22167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68942606"/>
+        <c:axId val="8636981"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22206,7 +22206,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23476956"/>
+        <c:crossAx val="18001325"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22258,7 +22258,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart212.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart255.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -22575,11 +22575,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="33902039"/>
-        <c:axId val="33812556"/>
+        <c:axId val="41884112"/>
+        <c:axId val="33702573"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="33902039"/>
+        <c:axId val="41884112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22611,14 +22611,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33812556"/>
+        <c:crossAx val="33702573"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33812556"/>
+        <c:axId val="33702573"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -22658,7 +22658,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33902039"/>
+        <c:crossAx val="41884112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22710,7 +22710,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart213.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart256.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -23027,11 +23027,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="11850109"/>
-        <c:axId val="55843550"/>
+        <c:axId val="5217051"/>
+        <c:axId val="32912235"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="11850109"/>
+        <c:axId val="5217051"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23063,14 +23063,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55843550"/>
+        <c:crossAx val="32912235"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55843550"/>
+        <c:axId val="32912235"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -23110,7 +23110,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11850109"/>
+        <c:crossAx val="5217051"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23162,7 +23162,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart214.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart257.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -23479,11 +23479,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="88219364"/>
-        <c:axId val="15667619"/>
+        <c:axId val="36712767"/>
+        <c:axId val="99108811"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88219364"/>
+        <c:axId val="36712767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23515,14 +23515,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15667619"/>
+        <c:crossAx val="99108811"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15667619"/>
+        <c:axId val="99108811"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -23562,7 +23562,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88219364"/>
+        <c:crossAx val="36712767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23614,7 +23614,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart215.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart258.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -23939,11 +23939,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="57051243"/>
-        <c:axId val="92487752"/>
+        <c:axId val="52975899"/>
+        <c:axId val="80981936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57051243"/>
+        <c:axId val="52975899"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23975,14 +23975,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92487752"/>
+        <c:crossAx val="80981936"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92487752"/>
+        <c:axId val="80981936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24021,7 +24021,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57051243"/>
+        <c:crossAx val="52975899"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24073,7 +24073,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -24407,7 +24407,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -24730,7 +24730,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -25053,7 +25053,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -25332,7 +25332,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -25611,7 +25611,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -29022,7 +29022,7 @@
   </sheetPr>
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>